<commit_message>
update readme for download links
</commit_message>
<xml_diff>
--- a/h3downpatch.xlsx
+++ b/h3downpatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\OneDrive\Documents\hitman-3-downpatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4CFF9D-77BC-462E-A5B7-969CF140542F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B2215C-6D94-417E-A542-11E35DDD0F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F95B05D7-EB20-4BD0-8CD4-1724CF9FC487}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Game Version</t>
   </si>
@@ -68,20 +68,190 @@
     <t>First Patch</t>
   </si>
   <si>
-    <t>Prompts don't work</t>
-  </si>
-  <si>
     <t>N/A (don't think Peacock is out yet</t>
+  </si>
+  <si>
+    <t>Prompts don't work (Fixed February 2021)</t>
+  </si>
+  <si>
+    <t>Eider 4466613</t>
+  </si>
+  <si>
+    <t>Eider 4472392</t>
+  </si>
+  <si>
+    <t>Eider 4564176</t>
+  </si>
+  <si>
+    <t>Eider 4635444</t>
+  </si>
+  <si>
+    <t>Eider 4685799</t>
+  </si>
+  <si>
+    <t>Eider 4763566</t>
+  </si>
+  <si>
+    <t>Eider 4879673</t>
+  </si>
+  <si>
+    <t>Eider 4916414</t>
+  </si>
+  <si>
+    <t>Eider 5010755</t>
+  </si>
+  <si>
+    <t>Eider 5086890</t>
+  </si>
+  <si>
+    <t>Eider 5191698</t>
+  </si>
+  <si>
+    <t>Eider 5220846</t>
+  </si>
+  <si>
+    <t>Eider 5259620</t>
+  </si>
+  <si>
+    <t>Eider 5527099</t>
+  </si>
+  <si>
+    <t>Eider 5540627</t>
+  </si>
+  <si>
+    <t>Eider 5561401</t>
+  </si>
+  <si>
+    <t>Eider 5898594</t>
+  </si>
+  <si>
+    <t>Eider 5915918</t>
+  </si>
+  <si>
+    <t>Eider 6041891</t>
+  </si>
+  <si>
+    <t>Eider 6239328</t>
+  </si>
+  <si>
+    <t>3.10.1 (OBS Hotfix - Assumed version number)</t>
+  </si>
+  <si>
+    <t>(contains no patches - GUESSED DATE 23rd on mine, 24th on yours)</t>
+  </si>
+  <si>
+    <t>3.11.0</t>
+  </si>
+  <si>
+    <t>3.20.0</t>
+  </si>
+  <si>
+    <t>Added "Retail/WinPixEventRuntime.dll"</t>
+  </si>
+  <si>
+    <t>3.20.1</t>
+  </si>
+  <si>
+    <t>(Frame Drop Patch - Assumed version number)</t>
+  </si>
+  <si>
+    <t>3.30.0</t>
+  </si>
+  <si>
+    <t>(Emetic Patch (sick NPC throw up elsewhere), Legal Accident Gaucho Sniper in Mendoza)</t>
+  </si>
+  <si>
+    <t>3.40.0</t>
+  </si>
+  <si>
+    <t>Introduction of patch2</t>
+  </si>
+  <si>
+    <t>3.40.1</t>
+  </si>
+  <si>
+    <t>(Overlay Patch)</t>
+  </si>
+  <si>
+    <t>3.50.0</t>
+  </si>
+  <si>
+    <t>3.50.1</t>
+  </si>
+  <si>
+    <t>3.70.0</t>
+  </si>
+  <si>
+    <t>3.70.1</t>
+  </si>
+  <si>
+    <t>("Woosh" fix - Version number didn't actually change)</t>
+  </si>
+  <si>
+    <t>Version number didn't actually change</t>
+  </si>
+  <si>
+    <t>3.70.2</t>
+  </si>
+  <si>
+    <t>3.100.0</t>
+  </si>
+  <si>
+    <t>3.100.1</t>
+  </si>
+  <si>
+    <t>(Y2 Hotfix - Version number didn't actually change)</t>
+  </si>
+  <si>
+    <t>3.100.2??</t>
+  </si>
+  <si>
+    <t>Seems to be a Y2 patch variant. No extra cameras in Master difficulty Dubai yet. May 19th according to featured contract thumbnails: https://www.hitmanforum.com/t/year-2-may-official-community-rubber-duck-featured-contracts/14702</t>
+  </si>
+  <si>
+    <t>3.100.3??</t>
+  </si>
+  <si>
+    <t>3.110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.120 </t>
+  </si>
+  <si>
+    <t>3.130</t>
+  </si>
+  <si>
+    <t>(S3 Master Cameras Patch, added invisible floor to Mendoza sliding roof) (need to confirm)</t>
+  </si>
+  <si>
+    <t>(Added Molly. Technically not the only patch with Molly playable)</t>
+  </si>
+  <si>
+    <t>(Removed molly accident / wallbang, changed NY frisk, changed Dartmoor ledge drop, removed RFID exploit)</t>
+  </si>
+  <si>
+    <t>(Year 2 Patch) Removed Dartmoor SA 37 chandy wallbang and fucked Romania doors</t>
+  </si>
+  <si>
+    <t>Introduction of patch1 (Removed Druzhina wallbang, train OOB, Berlin Manhole, Chongqing Vault Skip)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,14 +274,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,68 +607,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506407D6-E9B2-4B68-9011-EF7AE2674A2A}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="22.77734375" customWidth="1"/>
-    <col min="6" max="6" width="30.109375" customWidth="1"/>
-    <col min="7" max="7" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="3">
         <v>44216</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>11</v>
+    </row>
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>44217</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="3">
+        <v>44219</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3">
+        <v>44250</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3">
+        <v>44285</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3">
+        <v>44292</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3">
+        <v>44326</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3">
+        <v>44362</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3">
+        <v>44370</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3">
+        <v>44404</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>44439</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="3">
+        <v>44467</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="3">
+        <v>44470</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3">
+        <v>44495</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="3">
+        <v>44581</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="3">
+        <v>44582</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="3">
+        <v>44705</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="3">
+        <v>44705</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="3">
+        <v>44705</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3">
+        <v>44768</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="3">
+        <v>44840</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AFB4081E-4F43-4FA9-A025-1C2E07E00B47}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{A64C541C-DF9C-41B5-9432-59D6EC02032B}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{BAF78766-F532-4BCE-A98D-A7FC2C1BDAB2}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{B5AEE0A5-241D-4013-A344-9E0BCC7AACB6}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{222BAF93-E3A5-4072-8E92-80EFF8093577}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{416D6B8E-B00F-4FB0-A9D3-32AB3EEEF437}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{2CF74A34-487D-402B-82FB-C5133FD96D95}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{7C10CEDA-1ABC-415A-BBC3-0634055F989E}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{881F2B16-D521-4DB1-A819-1B42105F0A08}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{D1EB35E4-F3AD-43DC-88D1-44C5DBFFD3B7}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{81921CE4-7DC9-42B5-862F-A7D731ACA9FD}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{180B10AE-4596-4A52-86E7-349330CFC33D}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{D5664B1A-2237-47C8-882B-51EA8094EDCA}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{CFB82DBC-8798-4AF9-B6E8-61F97DA0C82C}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{BDE45A07-0FCA-4A61-AE60-150550D7995E}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{76BFB598-DF46-4962-89FC-51779522F95C}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{146D4D64-7B72-46B1-8052-31D30BC383A6}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{9E610823-2882-4A6F-90C8-86991B240869}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{F0B04CF7-5B84-4B1E-A494-1C428D2ACFCA}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{4B45458B-4D78-449C-9FEF-035FFE56AC06}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{EF213086-4043-4813-88C6-DD46E7AB0D38}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
see if bullets on the table work
</commit_message>
<xml_diff>
--- a/h3downpatch.xlsx
+++ b/h3downpatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\OneDrive\Documents\hitman-3-downpatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6D44C1-5013-4474-86D6-A1FF987719BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766249C7-5AE9-40D2-B5C1-FD4C80916B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F95B05D7-EB20-4BD0-8CD4-1724CF9FC487}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Game Version</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Release Date</t>
   </si>
   <si>
-    <t>First Patch</t>
-  </si>
-  <si>
     <t>Eider 4466613</t>
   </si>
   <si>
@@ -143,27 +140,6 @@
     <t>24-May-2022 or later</t>
   </si>
   <si>
-    <t>S3 Master Cameras Patch, added invisible floor to Mendoza sliding roof</t>
-  </si>
-  <si>
-    <t>Removed molly accident / wallbang, changed NY frisk, changed Dartmoor ledge drop, removed RFID exploit</t>
-  </si>
-  <si>
-    <t>Added Molly. Technically not the only patch with Molly playable</t>
-  </si>
-  <si>
-    <t>Removed Druzhina wallbang, train OOB, Berlin Manhole, Chongqing Vault Skip</t>
-  </si>
-  <si>
-    <t>Year 2 Patch. Removed Dartmoor SA 37 chandy wallbang and messed up sliding doors</t>
-  </si>
-  <si>
-    <t>Year 2 variant.</t>
-  </si>
-  <si>
-    <t>Year 2 variant. No extra cameras in Master difficulty Dubai yet. May 19th according to featured contract thumbnails: https://www.hitmanforum.com/t/year-2-may-official-community-rubber-duck-featured-contracts/14702</t>
-  </si>
-  <si>
     <t>Patch Note Commentary</t>
   </si>
   <si>
@@ -200,58 +176,88 @@
     <t>Somewhere between 20-Jan-2022 and 24-May-2022</t>
   </si>
   <si>
-    <t>Most recent ET Arcade dates to 2022-Jul-14</t>
-  </si>
-  <si>
     <t>https://www.ioi.dk/hitman-3-september-patch-3-70/</t>
   </si>
   <si>
     <t>https://www.ioi.dk/patch-notes-hitman3/</t>
   </si>
   <si>
-    <t xml:space="preserve">Check "October 1 - PC Only" in official patch notes. Fixed "No “Woosh” sound on PC. </t>
-  </si>
-  <si>
-    <t>Check "August 31 - PC Only" in official patch notes. Fixed an issue where players experienced FPS drops/ stuttering after the 3.50 (July) patch.</t>
-  </si>
-  <si>
     <t>https://www.ioi.dk/hitman-3-july-patch-3-50/</t>
   </si>
   <si>
-    <t>Added back shoulder swap. Tweaked sniper slowdown.</t>
-  </si>
-  <si>
-    <t>Check "June 21 - PC Only" in official patch notes. Fixed an issue with Epic Overlay.</t>
-  </si>
-  <si>
-    <t>Added Dartmoor game show</t>
-  </si>
-  <si>
     <t>https://www.ioi.dk/hitman-3-june-patch-3-40/</t>
   </si>
   <si>
     <t>https://www.ioi.dk/hitman-3-may-patch-3-30/</t>
   </si>
   <si>
-    <t>Emetic Patch (sick NPC throw up elsewhere), Legal Sniper in Mendoza (Gaucho Start) patched in Mendoza. Also some lighting fixes.</t>
-  </si>
-  <si>
     <t>https://www.ioi.dk/hitman-3-march-patch-3-20/</t>
   </si>
   <si>
-    <t>Check "April 6 - PC Only" in official patch notes. Fixed a frame rate issue.</t>
-  </si>
-  <si>
     <t>https://www.ioi.dk/hitman-3-february-patch-3-11/</t>
   </si>
   <si>
-    <t>Weird downpatch prompt issue fixed</t>
-  </si>
-  <si>
-    <t>First patch available to Steam users. First patch Molotov seems to be available.</t>
-  </si>
-  <si>
-    <t>Prompts UI is messed up (ON DOWNPATCHED VERSION, it was fine back in the day) (Fixed February 2021)</t>
+    <t>• Prompts UI is messed up (ON DOWNPATCHED VERSION, it was fine back in the day) (Fixed February 2021)</t>
+  </si>
+  <si>
+    <t>• Removed Druzhina wallbang
+• Removed Train OOB
+• Removed Berlin Manhole Exit
+• Removed a Chongqing Vault Skip
+• Weird downpatch prompt issue fixed</t>
+  </si>
+  <si>
+    <t>• First Patch. 
+• Prompts UI is messed up (ON DOWNPATCHED VERSION, it was fine back in the day) (Fixed February 2021)</t>
+  </si>
+  <si>
+    <t>• Check "April 6 - PC Only" in official patch notes. Fixed a frame rate issue.</t>
+  </si>
+  <si>
+    <t>• Emetic Patch (sick NPC throw up elsewhere), Legal Sniper in Mendoza (Gaucho Start) patched in Mendoza. Also some lighting fixes.</t>
+  </si>
+  <si>
+    <t>• Check "June 21 - PC Only" in official patch notes. Fixed an issue with Epic Overlay.</t>
+  </si>
+  <si>
+    <t>• Added Dartmoor game show</t>
+  </si>
+  <si>
+    <t>• Check "August 31 - PC Only" in official patch notes. Fixed an issue where players experienced FPS drops/ stuttering after the 3.50 (July) patch.</t>
+  </si>
+  <si>
+    <t>• Added back shoulder swap. Tweaked sniper slowdown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Check "October 1 - PC Only" in official patch notes. Fixed "No “Woosh” sound on PC. </t>
+  </si>
+  <si>
+    <t>• Year 2 Patch. Removed Dartmoor SA 37 chandy wallbang and messed up sliding doors
+• First patch available to Steam users.
+• First patch Molotov seems to be available.</t>
+  </si>
+  <si>
+    <t>• Year 2 variant.</t>
+  </si>
+  <si>
+    <t>• Year 2 variant. 
+• No extra cameras in Master difficulty Dubai yet. 
+• May 19th according to featured contract thumbnails: https://www.hitmanforum.com/t/year-2-may-official-community-rubber-duck-featured-contracts/14702</t>
+  </si>
+  <si>
+    <t>• S3 Master Cameras Patch
+• Added invisible floor to Mendoza sliding roof
+• Most recent ET Arcade dates to 2022-Jul-14</t>
+  </si>
+  <si>
+    <t>• Added Molotov. 
+• Technically not the only patch with Molly playable</t>
+  </si>
+  <si>
+    <t>• Removed molly accident / wallbang
+• Changed NY frisk
+• Changed Dartmoor ledge drop
+• Removed RFID exploit</t>
   </si>
 </sst>
 </file>
@@ -630,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506407D6-E9B2-4B68-9011-EF7AE2674A2A}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -657,16 +663,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -674,347 +680,332 @@
         <v>44216</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>44217</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>44219</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>44250</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3">
         <v>44285</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3">
         <v>44292</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3">
         <v>44326</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="3">
         <v>44362</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10" s="3">
         <v>44370</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>44404</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
         <v>44439</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3">
         <v>44467</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="3">
         <v>44470</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
         <v>44495</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>44581</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="3">
         <v>44582</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="B21" s="3">
         <v>44768</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="3">
         <v>44840</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
maybe switch to just markdown for table
</commit_message>
<xml_diff>
--- a/h3downpatch.xlsx
+++ b/h3downpatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Legion\OneDrive\Documents\hitman-3-downpatch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2209D1-BEF7-4FA7-9701-7EA7E7178F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B43210-D512-45F1-98F7-43FBF8024B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F95B05D7-EB20-4BD0-8CD4-1724CF9FC487}"/>
   </bookViews>
@@ -240,10 +240,6 @@
 • Most recent ET Arcade dates to 2022-Jul-14</t>
   </si>
   <si>
-    <t>• Added Molotov. 
-• Technically not the only patch with Molly playable</t>
-  </si>
-  <si>
     <t>• Removed molly accident / wallbang
 • Changed NY frisk
 • Changed Dartmoor ledge drop
@@ -258,6 +254,11 @@
     <t>• First Patch
 • Prompts UI is messed up (ON DOWNPATCHED VERSION, it was fine back in the day) 
   • (Fixed February 2021)</t>
+  </si>
+  <si>
+    <t>• Added Molotov. 
+• Technically not the only patch with Molly playable
+• Fixed (some) Haven viewcone wallhacks</t>
   </si>
 </sst>
 </file>
@@ -636,8 +637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{506407D6-E9B2-4B68-9011-EF7AE2674A2A}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,7 +681,7 @@
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -694,7 +695,7 @@
         <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -708,7 +709,7 @@
         <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
@@ -971,7 +972,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -985,7 +986,7 @@
         <v>42</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
@@ -1002,7 +1003,7 @@
         <v>36</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>